<commit_message>
se sube para hacer smoke en QA R32
</commit_message>
<xml_diff>
--- a/Smoke/DataSource - Emision Motor.xlsx
+++ b/Smoke/DataSource - Emision Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DD5B9D-FD2E-4510-B3AE-8A4A9DAEBFF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41E2CB4-D7CF-45F8-A436-EEA548C19BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>CPremium - Resp. Civil-Robo/Incendio Total y Parcial Daños Totales por Accidente</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>CodInfoAuto</t>
+  </si>
+  <si>
+    <t>TR - Todo Riesgo Franquicia Fija</t>
   </si>
 </sst>
 </file>
@@ -222,13 +222,13 @@
       <sheetData sheetId="2">
         <row r="2">
           <cell r="A2" t="str">
-            <v>PRC015</v>
+            <v>SMA002</v>
           </cell>
           <cell r="B2" t="str">
-            <v>ABC12SPRC015</v>
+            <v>ABC12SSMA002</v>
           </cell>
           <cell r="C2" t="str">
-            <v>ZAZ123SPRC015</v>
+            <v>ZAZ123SSMA002</v>
           </cell>
         </row>
       </sheetData>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z503"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,10 +577,10 @@
         <v>5</v>
       </c>
       <c r="P1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R1" t="s">
         <v>6</v>
@@ -607,7 +607,7 @@
         <v>13</v>
       </c>
       <c r="Z1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -619,14 +619,14 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O2">
         <v>2021</v>
@@ -635,28 +635,28 @@
         <v>180698</v>
       </c>
       <c r="Q2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="V2" t="str">
         <f>[1]DatosMotor!$A$2</f>
-        <v>PRC015</v>
+        <v>SMA002</v>
       </c>
       <c r="W2" t="str">
         <f>[1]DatosMotor!$B$2</f>
-        <v>ABC12SPRC015</v>
+        <v>ABC12SSMA002</v>
       </c>
       <c r="X2" t="str">
         <f>[1]DatosMotor!$C$2</f>
-        <v>ZAZ123SPRC015</v>
+        <v>ZAZ123SSMA002</v>
       </c>
       <c r="Y2" t="s">
         <v>15</v>
       </c>
       <c r="Z2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
pruebaDecima de creacin de cuenta
</commit_message>
<xml_diff>
--- a/Smoke/DataSource - Emision Motor.xlsx
+++ b/Smoke/DataSource - Emision Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41E2CB4-D7CF-45F8-A436-EEA548C19BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C004400-B28C-4B0A-A65E-E31DEE4138F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>NroCuenta</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>TR - Todo Riesgo Franquicia Fija</t>
+  </si>
+  <si>
+    <t>FORD</t>
+  </si>
+  <si>
+    <t>ECO SPORT 1.5 SE AUT L/18</t>
+  </si>
+  <si>
+    <t>KA 1.5 FREESTYLE SEL AT6 L/18</t>
   </si>
 </sst>
 </file>
@@ -222,13 +231,13 @@
       <sheetData sheetId="2">
         <row r="2">
           <cell r="A2" t="str">
-            <v>SMA002</v>
+            <v>SMA007</v>
           </cell>
           <cell r="B2" t="str">
-            <v>ABC12SSMA002</v>
+            <v>ABC12SSMA007</v>
           </cell>
           <cell r="C2" t="str">
-            <v>ZAZ123SSMA002</v>
+            <v>ZAZ123SSMA007</v>
           </cell>
         </row>
       </sheetData>
@@ -503,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z503"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +641,7 @@
         <v>2021</v>
       </c>
       <c r="P2">
-        <v>180698</v>
+        <v>180725</v>
       </c>
       <c r="Q2" t="s">
         <v>28</v>
@@ -642,15 +651,15 @@
       </c>
       <c r="V2" t="str">
         <f>[1]DatosMotor!$A$2</f>
-        <v>SMA002</v>
+        <v>SMA007</v>
       </c>
       <c r="W2" t="str">
         <f>[1]DatosMotor!$B$2</f>
-        <v>ABC12SSMA002</v>
+        <v>ABC12SSMA007</v>
       </c>
       <c r="X2" t="str">
         <f>[1]DatosMotor!$C$2</f>
-        <v>ZAZ123SSMA002</v>
+        <v>ZAZ123SSMA007</v>
       </c>
       <c r="Y2" t="s">
         <v>15</v>
@@ -666,14 +675,35 @@
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="F4" s="1"/>
+      <c r="P4">
+        <v>180698</v>
+      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="F5" s="1"/>
+      <c r="P5">
+        <v>180696</v>
+      </c>
+      <c r="R5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="F6" s="1"/>
+      <c r="P6">
+        <v>180725</v>
+      </c>
+      <c r="R6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7"/>

</xml_diff>

<commit_message>
se sube para hacer Smoke de nuevo
</commit_message>
<xml_diff>
--- a/Smoke/DataSource - Emision Motor.xlsx
+++ b/Smoke/DataSource - Emision Motor.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C004400-B28C-4B0A-A65E-E31DEE4138F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7335442B-5657-4939-9A4D-3F85E0DAA18C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -513,7 +514,7 @@
   <dimension ref="A1:Z503"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,35 +676,14 @@
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="F4" s="1"/>
-      <c r="P4">
-        <v>180698</v>
-      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="F5" s="1"/>
-      <c r="P5">
-        <v>180696</v>
-      </c>
-      <c r="R5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S5" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="F6" s="1"/>
-      <c r="P6">
-        <v>180725</v>
-      </c>
-      <c r="R6" t="s">
-        <v>32</v>
-      </c>
-      <c r="S6" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="7" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7"/>
@@ -3394,4 +3374,46 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C738C0CF-ABFE-486A-94BD-6F53840A5E94}">
+  <dimension ref="B2:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>180698</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>180696</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>180725</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se agrega getValue del año actual del ambiente para emisión de Autos
</commit_message>
<xml_diff>
--- a/Smoke/DataSource - Emision Motor.xlsx
+++ b/Smoke/DataSource - Emision Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7335442B-5657-4939-9A4D-3F85E0DAA18C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB1188E-35C5-41D0-BCCD-4E394F72B61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>NroCuenta</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>OPCION_PAGOCUOTAS</t>
-  </si>
-  <si>
-    <t>Anio</t>
   </si>
   <si>
     <t>Marca</t>
@@ -232,13 +229,13 @@
       <sheetData sheetId="2">
         <row r="2">
           <cell r="A2" t="str">
-            <v>SMA007</v>
+            <v>SMP035</v>
           </cell>
           <cell r="B2" t="str">
-            <v>ABC12SSMA007</v>
+            <v>ABC12SSMP035</v>
           </cell>
           <cell r="C2" t="str">
-            <v>ZAZ123SSMA007</v>
+            <v>ZAZ123SSMP035</v>
           </cell>
         </row>
       </sheetData>
@@ -511,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z503"/>
+  <dimension ref="A1:Y503"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,24 +522,24 @@
     <col min="4" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="14" width="21.28515625" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" customWidth="1"/>
-    <col min="19" max="19" width="18" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
-    <col min="21" max="21" width="22.42578125" customWidth="1"/>
-    <col min="22" max="22" width="21.85546875" customWidth="1"/>
-    <col min="23" max="23" width="17.140625" customWidth="1"/>
-    <col min="24" max="24" width="17.7109375" customWidth="1"/>
-    <col min="25" max="25" width="12.42578125" customWidth="1"/>
-    <col min="26" max="26" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="21.28515625" customWidth="1"/>
+    <col min="14" max="14" width="21.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="18" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" customWidth="1"/>
+    <col min="20" max="20" width="22.42578125" customWidth="1"/>
+    <col min="21" max="21" width="21.85546875" customWidth="1"/>
+    <col min="22" max="22" width="17.140625" customWidth="1"/>
+    <col min="23" max="23" width="17.7109375" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" customWidth="1"/>
+    <col min="25" max="25" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -554,10 +551,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -566,31 +563,31 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" t="s">
-        <v>23</v>
-      </c>
       <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
         <v>5</v>
-      </c>
-      <c r="P1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>27</v>
       </c>
       <c r="R1" t="s">
         <v>6</v>
@@ -614,78 +611,72 @@
         <v>12</v>
       </c>
       <c r="Y1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2">
+        <v>180725</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2" t="str">
+        <f>[1]DatosMotor!$A$2</f>
+        <v>SMP035</v>
+      </c>
+      <c r="V2" t="str">
+        <f>[1]DatosMotor!$B$2</f>
+        <v>ABC12SSMP035</v>
+      </c>
+      <c r="W2" t="str">
+        <f>[1]DatosMotor!$C$2</f>
+        <v>ZAZ123SSMP035</v>
+      </c>
+      <c r="X2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2">
-        <v>2021</v>
-      </c>
-      <c r="P2">
-        <v>180725</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>28</v>
-      </c>
-      <c r="U2" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" t="str">
-        <f>[1]DatosMotor!$A$2</f>
-        <v>SMA007</v>
-      </c>
-      <c r="W2" t="str">
-        <f>[1]DatosMotor!$B$2</f>
-        <v>ABC12SSMA007</v>
-      </c>
-      <c r="X2" t="str">
-        <f>[1]DatosMotor!$C$2</f>
-        <v>ZAZ123SSMA007</v>
-      </c>
       <c r="Y2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7" s="3"/>
       <c r="C7"/>
@@ -711,9 +702,8 @@
       <c r="W7"/>
       <c r="X7"/>
       <c r="Y7"/>
-      <c r="Z7"/>
-    </row>
-    <row r="8" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8"/>
       <c r="B8" s="3"/>
       <c r="C8"/>
@@ -739,9 +729,8 @@
       <c r="W8"/>
       <c r="X8"/>
       <c r="Y8"/>
-      <c r="Z8"/>
-    </row>
-    <row r="9" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9"/>
       <c r="B9" s="3"/>
       <c r="C9"/>
@@ -767,9 +756,8 @@
       <c r="W9"/>
       <c r="X9"/>
       <c r="Y9"/>
-      <c r="Z9"/>
-    </row>
-    <row r="10" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10" s="3"/>
       <c r="C10"/>
@@ -795,9 +783,8 @@
       <c r="W10"/>
       <c r="X10"/>
       <c r="Y10"/>
-      <c r="Z10"/>
-    </row>
-    <row r="11" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11" s="3"/>
       <c r="C11"/>
@@ -823,9 +810,8 @@
       <c r="W11"/>
       <c r="X11"/>
       <c r="Y11"/>
-      <c r="Z11"/>
-    </row>
-    <row r="12" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12" s="3"/>
       <c r="C12"/>
@@ -851,9 +837,8 @@
       <c r="W12"/>
       <c r="X12"/>
       <c r="Y12"/>
-      <c r="Z12"/>
-    </row>
-    <row r="13" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13" s="3"/>
       <c r="C13"/>
@@ -879,57 +864,56 @@
       <c r="W13"/>
       <c r="X13"/>
       <c r="Y13"/>
-      <c r="Z13"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26" s="3"/>
       <c r="C26"/>
@@ -955,9 +939,8 @@
       <c r="W26"/>
       <c r="X26"/>
       <c r="Y26"/>
-      <c r="Z26"/>
-    </row>
-    <row r="27" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27" s="3"/>
       <c r="C27"/>
@@ -983,57 +966,56 @@
       <c r="W27"/>
       <c r="X27"/>
       <c r="Y27"/>
-      <c r="Z27"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40" s="3"/>
       <c r="C40"/>
@@ -1059,9 +1041,8 @@
       <c r="W40"/>
       <c r="X40"/>
       <c r="Y40"/>
-      <c r="Z40"/>
-    </row>
-    <row r="41" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41" s="3"/>
       <c r="C41"/>
@@ -1087,9 +1068,8 @@
       <c r="W41"/>
       <c r="X41"/>
       <c r="Y41"/>
-      <c r="Z41"/>
-    </row>
-    <row r="42" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42" s="3"/>
       <c r="C42"/>
@@ -1115,9 +1095,8 @@
       <c r="W42"/>
       <c r="X42"/>
       <c r="Y42"/>
-      <c r="Z42"/>
-    </row>
-    <row r="43" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43" s="3"/>
       <c r="C43"/>
@@ -1143,9 +1122,8 @@
       <c r="W43"/>
       <c r="X43"/>
       <c r="Y43"/>
-      <c r="Z43"/>
-    </row>
-    <row r="44" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44" s="3"/>
       <c r="C44"/>
@@ -1171,9 +1149,8 @@
       <c r="W44"/>
       <c r="X44"/>
       <c r="Y44"/>
-      <c r="Z44"/>
-    </row>
-    <row r="45" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45" s="3"/>
       <c r="C45"/>
@@ -1199,9 +1176,8 @@
       <c r="W45"/>
       <c r="X45"/>
       <c r="Y45"/>
-      <c r="Z45"/>
-    </row>
-    <row r="46" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46" s="3"/>
       <c r="C46"/>
@@ -1227,9 +1203,8 @@
       <c r="W46"/>
       <c r="X46"/>
       <c r="Y46"/>
-      <c r="Z46"/>
-    </row>
-    <row r="47" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47" s="3"/>
       <c r="C47"/>
@@ -1255,57 +1230,56 @@
       <c r="W47"/>
       <c r="X47"/>
       <c r="Y47"/>
-      <c r="Z47"/>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60" s="3"/>
       <c r="C60"/>
@@ -1331,9 +1305,8 @@
       <c r="W60"/>
       <c r="X60"/>
       <c r="Y60"/>
-      <c r="Z60"/>
-    </row>
-    <row r="61" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61" s="3"/>
       <c r="C61"/>
@@ -1359,57 +1332,56 @@
       <c r="W61"/>
       <c r="X61"/>
       <c r="Y61"/>
-      <c r="Z61"/>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B64" s="3"/>
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B66" s="3"/>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B70" s="3"/>
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B71" s="3"/>
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B72" s="3"/>
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B73" s="3"/>
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74"/>
       <c r="B74" s="3"/>
       <c r="C74"/>
@@ -1435,9 +1407,8 @@
       <c r="W74"/>
       <c r="X74"/>
       <c r="Y74"/>
-      <c r="Z74"/>
-    </row>
-    <row r="75" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75"/>
       <c r="B75" s="3"/>
       <c r="C75"/>
@@ -1463,9 +1434,8 @@
       <c r="W75"/>
       <c r="X75"/>
       <c r="Y75"/>
-      <c r="Z75"/>
-    </row>
-    <row r="76" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76"/>
       <c r="B76" s="3"/>
       <c r="C76"/>
@@ -1491,9 +1461,8 @@
       <c r="W76"/>
       <c r="X76"/>
       <c r="Y76"/>
-      <c r="Z76"/>
-    </row>
-    <row r="77" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77"/>
       <c r="B77" s="3"/>
       <c r="C77"/>
@@ -1519,9 +1488,8 @@
       <c r="W77"/>
       <c r="X77"/>
       <c r="Y77"/>
-      <c r="Z77"/>
-    </row>
-    <row r="78" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78"/>
       <c r="B78" s="3"/>
       <c r="C78"/>
@@ -1547,9 +1515,8 @@
       <c r="W78"/>
       <c r="X78"/>
       <c r="Y78"/>
-      <c r="Z78"/>
-    </row>
-    <row r="79" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79"/>
       <c r="B79" s="3"/>
       <c r="C79"/>
@@ -1575,9 +1542,8 @@
       <c r="W79"/>
       <c r="X79"/>
       <c r="Y79"/>
-      <c r="Z79"/>
-    </row>
-    <row r="80" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80"/>
       <c r="B80" s="3"/>
       <c r="C80"/>
@@ -1603,9 +1569,8 @@
       <c r="W80"/>
       <c r="X80"/>
       <c r="Y80"/>
-      <c r="Z80"/>
-    </row>
-    <row r="81" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81"/>
       <c r="B81" s="3"/>
       <c r="C81"/>
@@ -1631,57 +1596,56 @@
       <c r="W81"/>
       <c r="X81"/>
       <c r="Y81"/>
-      <c r="Z81"/>
-    </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B82" s="3"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B83" s="3"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B84" s="3"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B85" s="3"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B86" s="3"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B87" s="3"/>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B88" s="3"/>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B89" s="3"/>
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B90" s="3"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B91" s="3"/>
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B92" s="3"/>
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B93" s="3"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94"/>
       <c r="B94" s="3"/>
       <c r="C94"/>
@@ -1707,9 +1671,8 @@
       <c r="W94"/>
       <c r="X94"/>
       <c r="Y94"/>
-      <c r="Z94"/>
-    </row>
-    <row r="95" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95"/>
       <c r="B95" s="3"/>
       <c r="C95"/>
@@ -1735,9 +1698,8 @@
       <c r="W95"/>
       <c r="X95"/>
       <c r="Y95"/>
-      <c r="Z95"/>
-    </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B96" s="3"/>
       <c r="F96" s="1"/>
     </row>
@@ -3396,10 +3358,10 @@
         <v>180696</v>
       </c>
       <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -3407,10 +3369,10 @@
         <v>180725</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregó modelo FIAT 147 y suma segurada
</commit_message>
<xml_diff>
--- a/Smoke/DataSource - Emision Motor.xlsx
+++ b/Smoke/DataSource - Emision Motor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Smoke\Smoke\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB1188E-35C5-41D0-BCCD-4E394F72B61E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E7CD8A-F7D0-4733-8BD9-D64018024B1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,10 +633,13 @@
         <v>24</v>
       </c>
       <c r="O2">
-        <v>180725</v>
+        <v>179912</v>
       </c>
       <c r="P2" t="s">
         <v>27</v>
+      </c>
+      <c r="S2">
+        <v>1100000</v>
       </c>
       <c r="T2" t="s">
         <v>30</v>

</xml_diff>